<commit_message>
- Update requirement and design for summary reports
</commit_message>
<xml_diff>
--- a/Tags/Document/OrderDesign.xlsx
+++ b/Tags/Document/OrderDesign.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="135">
   <si>
     <t>Hóa đơn bán hàng</t>
   </si>
@@ -264,6 +264,171 @@
   </si>
   <si>
     <t xml:space="preserve">Tổng = </t>
+  </si>
+  <si>
+    <t>Tồn đầu kỳ</t>
+  </si>
+  <si>
+    <t>Xuất Trong kỳ</t>
+  </si>
+  <si>
+    <t>Nhập Trong kỳ</t>
+  </si>
+  <si>
+    <t>Tồn cuối kỳ</t>
+  </si>
+  <si>
+    <t>Danh sách các hóa đơn</t>
+  </si>
+  <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>Mã Hóa Đơn</t>
+  </si>
+  <si>
+    <t>Tên khách</t>
+  </si>
+  <si>
+    <t>Diễn Giải (Xuất | Nhập)</t>
+  </si>
+  <si>
+    <t>Số Lượng Nhập</t>
+  </si>
+  <si>
+    <t>Báo cáo chi tiết</t>
+  </si>
+  <si>
+    <t>Trong báo cáo lỗ lãi, thay số lượng bằng tiền</t>
+  </si>
+  <si>
+    <t>Tổng tiền thu</t>
+  </si>
+  <si>
+    <t>Tổng tiền chi</t>
+  </si>
+  <si>
+    <t>Thu Trong kỳ</t>
+  </si>
+  <si>
+    <t>Diễn Giải (Xuat | Thanh Toán | Chi)</t>
+  </si>
+  <si>
+    <t>Tổng tiền thanh toán (thu)</t>
+  </si>
+  <si>
+    <t>HDXuat</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>HDThanhToan</t>
+  </si>
+  <si>
+    <t>PhieuChi</t>
+  </si>
+  <si>
+    <t>Công Nợ khách hàng (chi tiết)</t>
+  </si>
+  <si>
+    <t>Công nợ khách hàng</t>
+  </si>
+  <si>
+    <t>Mã KH</t>
+  </si>
+  <si>
+    <t>Tên KH</t>
+  </si>
+  <si>
+    <t>Xuất trong kì</t>
+  </si>
+  <si>
+    <t>Thanh toán trong kì</t>
+  </si>
+  <si>
+    <t>Tồn cuối kì</t>
+  </si>
+  <si>
+    <t>Tồn Đầu Kì</t>
+  </si>
+  <si>
+    <t>Công nợ nhà cung cấp</t>
+  </si>
+  <si>
+    <t>Công nợ nhà cung cấp - chi tiết</t>
+  </si>
+  <si>
+    <t>Diễn Giải (Nhập | Thanh Toán | Chi)</t>
+  </si>
+  <si>
+    <t>HDNhập</t>
+  </si>
+  <si>
+    <t>Mã hóa đơn</t>
+  </si>
+  <si>
+    <t>Tên Khách</t>
+  </si>
+  <si>
+    <t>Diễn giải (xuất)</t>
+  </si>
+  <si>
+    <t>Tổng tiền</t>
+  </si>
+  <si>
+    <t>Doanh thu (tổng tiền của tất cả hóa đơn)</t>
+  </si>
+  <si>
+    <t>Tổng tiền chi + xuất (mình xuất hàng cho họ)</t>
+  </si>
+  <si>
+    <t>Tổng tiền thu + nhập (mình nhập hàng của họ)</t>
+  </si>
+  <si>
+    <t>Tổng tiền thanh toán (chi) - mình thanh toán cho họ</t>
+  </si>
+  <si>
+    <t>Tổng tiền nhập (tổng tiền của tất cả hóa đơn)</t>
+  </si>
+  <si>
+    <t>Diễn giải (nhập)</t>
+  </si>
+  <si>
+    <t>Báo cáo doanh thu - xem mình bán bao nhiêu tiền 1 tháng</t>
+  </si>
+  <si>
+    <t>Báo cáo hàng nhập - xem mình nhập bao nhiêu tiền 1 tháng</t>
+  </si>
+  <si>
+    <t>Báo cáo tiền mặt</t>
+  </si>
+  <si>
+    <t>Tồn đầu kì (tiền đầu ngày của kỳ truy vấn)</t>
+  </si>
+  <si>
+    <t>Thu trong kì (tổng phiếu thu trong kỳ)</t>
+  </si>
+  <si>
+    <t>Chi trong kì (tổng phiếu chi)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tồn cuối kì </t>
+  </si>
+  <si>
+    <t>Mã phiếu</t>
+  </si>
+  <si>
+    <t>PHIEUTHU</t>
+  </si>
+  <si>
+    <t>PHEUCHI</t>
+  </si>
+  <si>
+    <t>Tinh toan dua tren so luong xuat trung binh mot tuan (= 0 hoặc nhỏ hơn 1 con số nào đấy) de thong bao so luong hang can dat</t>
+  </si>
+  <si>
+    <t>Module ho tro dat hang - nghiên cứu</t>
   </si>
 </sst>
 </file>
@@ -400,7 +565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -432,10 +597,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -444,8 +615,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -826,19 +1012,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S109"/>
+  <dimension ref="A1:S189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="B189" sqref="B189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -1083,15 +1271,15 @@
       <c r="F13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="24" t="s">
+      <c r="G13" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="23" t="s">
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="K13" s="23"/>
+      <c r="K13" s="26"/>
       <c r="L13" s="16" t="s">
         <v>41</v>
       </c>
@@ -1111,7 +1299,7 @@
       <c r="R13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="S13" s="27" t="s">
+      <c r="S13" s="24" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1175,11 +1363,11 @@
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
       <c r="L20" s="12"/>
-      <c r="M20" s="25" t="s">
+      <c r="M20" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
@@ -2198,11 +2386,720 @@
       <c r="E109" s="8"/>
       <c r="F109" s="9"/>
     </row>
+    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D112" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="E112" s="30"/>
+      <c r="F112" s="30"/>
+    </row>
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B113" s="1"/>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G113" s="2">
+        <v>3</v>
+      </c>
+      <c r="H113" s="3"/>
+    </row>
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B114" s="4"/>
+      <c r="C114" s="5"/>
+      <c r="D114" s="5"/>
+      <c r="E114" s="5"/>
+      <c r="F114" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G114" s="5"/>
+      <c r="H114" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B115" s="4"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="5"/>
+      <c r="E115" s="5"/>
+      <c r="F115" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G115" s="5">
+        <v>2</v>
+      </c>
+      <c r="H115" s="6"/>
+    </row>
+    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B116" s="4"/>
+      <c r="C116" s="5"/>
+      <c r="D116" s="5"/>
+      <c r="E116" s="5"/>
+      <c r="F116" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G116" s="5">
+        <v>3</v>
+      </c>
+      <c r="H116" s="6"/>
+    </row>
+    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B117" s="4"/>
+      <c r="C117" s="5"/>
+      <c r="D117" s="5"/>
+      <c r="E117" s="5"/>
+      <c r="F117" s="5"/>
+      <c r="G117" s="5"/>
+      <c r="H117" s="6"/>
+    </row>
+    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B118" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C118" s="5"/>
+      <c r="D118" s="5"/>
+      <c r="E118" s="5"/>
+      <c r="F118" s="5"/>
+      <c r="G118" s="5"/>
+      <c r="H118" s="6"/>
+    </row>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B119" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E119" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F119" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G119" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H119" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B120" s="7"/>
+      <c r="C120" s="8"/>
+      <c r="D120" s="8"/>
+      <c r="E120" s="8"/>
+      <c r="F120" s="8"/>
+      <c r="G120" s="8"/>
+      <c r="H120" s="9"/>
+    </row>
+    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G122" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E125" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B127" s="1"/>
+      <c r="C127" s="2"/>
+      <c r="D127" s="2"/>
+      <c r="E127" s="2"/>
+      <c r="F127" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G127" s="2">
+        <v>3000</v>
+      </c>
+      <c r="H127" s="3"/>
+    </row>
+    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B128" s="4"/>
+      <c r="C128" s="5"/>
+      <c r="D128" s="5"/>
+      <c r="E128" s="5"/>
+      <c r="F128" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G128" s="5"/>
+      <c r="H128" s="6">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B129" s="4"/>
+      <c r="C129" s="5"/>
+      <c r="D129" s="5"/>
+      <c r="E129" s="5"/>
+      <c r="F129" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G129" s="5">
+        <v>2000</v>
+      </c>
+      <c r="H129" s="6"/>
+    </row>
+    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B130" s="4"/>
+      <c r="C130" s="5"/>
+      <c r="D130" s="5"/>
+      <c r="E130" s="5"/>
+      <c r="F130" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G130" s="5">
+        <v>3000</v>
+      </c>
+      <c r="H130" s="6"/>
+    </row>
+    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B131" s="4"/>
+      <c r="C131" s="5"/>
+      <c r="D131" s="5"/>
+      <c r="E131" s="5"/>
+      <c r="F131" s="5"/>
+      <c r="G131" s="5"/>
+      <c r="H131" s="6"/>
+    </row>
+    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B132" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C132" s="5"/>
+      <c r="D132" s="5"/>
+      <c r="E132" s="5"/>
+      <c r="F132" s="5"/>
+      <c r="G132" s="5"/>
+      <c r="H132" s="6"/>
+    </row>
+    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B133" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D133" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E133" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F133" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G133" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H133" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B134" s="7">
+        <v>1</v>
+      </c>
+      <c r="C134" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D134" s="8"/>
+      <c r="E134" s="8"/>
+      <c r="F134" s="8"/>
+      <c r="G134" s="8"/>
+      <c r="H134" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B135">
+        <v>2</v>
+      </c>
+      <c r="C135" t="s">
+        <v>99</v>
+      </c>
+      <c r="G135" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B136">
+        <v>3</v>
+      </c>
+      <c r="C136" t="s">
+        <v>100</v>
+      </c>
+      <c r="H136" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E138" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="139" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B139" s="1"/>
+      <c r="C139" s="2"/>
+      <c r="D139" s="2"/>
+      <c r="E139" s="2"/>
+      <c r="F139" s="2"/>
+      <c r="G139" s="2"/>
+      <c r="H139" s="3"/>
+    </row>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B140" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C140" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D140" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E140" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F140" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G140" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H140" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="141" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B141" s="7"/>
+      <c r="C141" s="8"/>
+      <c r="D141" s="8"/>
+      <c r="E141" s="8"/>
+      <c r="F141" s="8"/>
+      <c r="G141" s="8"/>
+      <c r="H141" s="9"/>
+    </row>
+    <row r="144" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E144" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="146" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B146" s="1"/>
+      <c r="C146" s="2"/>
+      <c r="D146" s="2"/>
+      <c r="E146" s="2"/>
+      <c r="F146" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G146" s="2">
+        <v>3000</v>
+      </c>
+      <c r="H146" s="3"/>
+    </row>
+    <row r="147" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B147" s="4"/>
+      <c r="C147" s="5"/>
+      <c r="D147" s="5"/>
+      <c r="E147" s="5"/>
+      <c r="F147" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G147" s="5"/>
+      <c r="H147" s="6">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="148" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B148" s="4"/>
+      <c r="C148" s="5"/>
+      <c r="D148" s="5"/>
+      <c r="E148" s="5"/>
+      <c r="F148" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G148" s="5">
+        <v>2000</v>
+      </c>
+      <c r="H148" s="6"/>
+    </row>
+    <row r="149" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B149" s="4"/>
+      <c r="C149" s="5"/>
+      <c r="D149" s="5"/>
+      <c r="E149" s="5"/>
+      <c r="F149" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G149" s="5">
+        <v>3000</v>
+      </c>
+      <c r="H149" s="6"/>
+    </row>
+    <row r="150" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B150" s="4"/>
+      <c r="C150" s="5"/>
+      <c r="D150" s="5"/>
+      <c r="E150" s="5"/>
+      <c r="F150" s="5"/>
+      <c r="G150" s="5"/>
+      <c r="H150" s="6"/>
+    </row>
+    <row r="151" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B151" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C151" s="5"/>
+      <c r="D151" s="5"/>
+      <c r="E151" s="5"/>
+      <c r="F151" s="5"/>
+      <c r="G151" s="5"/>
+      <c r="H151" s="6"/>
+    </row>
+    <row r="152" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B152" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C152" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D152" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E152" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F152" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G152" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H152" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="153" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B153" s="7">
+        <v>1</v>
+      </c>
+      <c r="C153" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D153" s="8"/>
+      <c r="E153" s="8"/>
+      <c r="F153" s="8"/>
+      <c r="G153" s="8"/>
+      <c r="H153" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="154" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B154" s="4">
+        <v>2</v>
+      </c>
+      <c r="C154" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D154" s="5"/>
+      <c r="E154" s="5"/>
+      <c r="F154" s="5"/>
+      <c r="G154" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H154" s="6"/>
+    </row>
+    <row r="155" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B155" s="7">
+        <v>3</v>
+      </c>
+      <c r="C155" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D155" s="8"/>
+      <c r="E155" s="8"/>
+      <c r="F155" s="8"/>
+      <c r="G155" s="8"/>
+      <c r="H155" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="157" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E157" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="158" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B158" s="1"/>
+      <c r="C158" s="2"/>
+      <c r="D158" s="2"/>
+      <c r="E158" s="2"/>
+      <c r="F158" s="2"/>
+      <c r="G158" s="2"/>
+      <c r="H158" s="3"/>
+    </row>
+    <row r="159" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B159" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C159" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D159" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E159" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F159" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="G159" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="H159" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="164" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E164" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="165" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B165" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C165" s="2"/>
+      <c r="D165" s="2"/>
+      <c r="F165" s="2"/>
+      <c r="G165" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="166" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B166" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C166" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D166" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E166" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F166" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G166" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="167" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B167" s="7"/>
+      <c r="C167" s="8"/>
+      <c r="D167" s="8"/>
+      <c r="E167" s="8"/>
+      <c r="F167" s="8"/>
+      <c r="G167" s="9"/>
+    </row>
+    <row r="169" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E169" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="170" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B170" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C170" s="2"/>
+      <c r="D170" s="2"/>
+      <c r="E170" s="2"/>
+      <c r="F170" s="2"/>
+      <c r="G170" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="171" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B171" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C171" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D171" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E171" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F171" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G171" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="172" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B172" s="7"/>
+      <c r="C172" s="8"/>
+      <c r="D172" s="8"/>
+      <c r="E172" s="8"/>
+      <c r="F172" s="8"/>
+      <c r="G172" s="9"/>
+    </row>
+    <row r="175" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E175" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="176" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B176" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C176" s="2"/>
+      <c r="D176" s="2"/>
+      <c r="E176" s="2"/>
+      <c r="F176" s="2"/>
+      <c r="G176" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="H176" s="32"/>
+    </row>
+    <row r="177" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B177" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C177" s="5"/>
+      <c r="D177" s="5"/>
+      <c r="E177" s="5"/>
+      <c r="F177" s="5"/>
+      <c r="G177" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="H177" s="6"/>
+    </row>
+    <row r="178" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B178" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C178" s="5"/>
+      <c r="D178" s="5"/>
+      <c r="E178" s="5"/>
+      <c r="F178" s="5"/>
+      <c r="G178" s="5"/>
+      <c r="H178" s="33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="179" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B179" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C179" s="5"/>
+      <c r="D179" s="5"/>
+      <c r="E179" s="5"/>
+      <c r="F179" s="5"/>
+      <c r="G179" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="H179" s="34"/>
+    </row>
+    <row r="180" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B180" s="4"/>
+      <c r="C180" s="5"/>
+      <c r="D180" s="5"/>
+      <c r="E180" s="5"/>
+      <c r="F180" s="5"/>
+      <c r="G180" s="5"/>
+      <c r="H180" s="6"/>
+    </row>
+    <row r="181" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B181" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C181" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D181" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E181" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F181" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G181" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H181" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="182" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B182" s="4"/>
+      <c r="C182" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D182" s="5"/>
+      <c r="E182" s="5"/>
+      <c r="F182" s="5"/>
+      <c r="G182" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="H182" s="6"/>
+    </row>
+    <row r="183" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B183" s="4"/>
+      <c r="C183" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D183" s="5"/>
+      <c r="E183" s="5"/>
+      <c r="F183" s="5"/>
+      <c r="G183" s="5"/>
+      <c r="H183" s="33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="184" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B184" s="7"/>
+      <c r="C184" s="8"/>
+      <c r="D184" s="8"/>
+      <c r="E184" s="8"/>
+      <c r="F184" s="8"/>
+      <c r="G184" s="8"/>
+      <c r="H184" s="9"/>
+    </row>
+    <row r="188" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B188" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="C188" s="29"/>
+    </row>
+    <row r="189" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B189" t="s">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
+    <mergeCell ref="G179:H179"/>
+    <mergeCell ref="B188:C188"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="M20:O20"/>
+    <mergeCell ref="D112:F112"/>
+    <mergeCell ref="G176:H176"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
- Create coupon management - Update some constraints: from now, customer is not null for order, coupon and bills
</commit_message>
<xml_diff>
--- a/Tags/Document/OrderDesign.xlsx
+++ b/Tags/Document/OrderDesign.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="136">
   <si>
     <t>Hóa đơn bán hàng</t>
   </si>
@@ -429,6 +429,9 @@
   </si>
   <si>
     <t>Module ho tro dat hang - nghiên cứu</t>
+  </si>
+  <si>
+    <t>Báo Cáo Lỗ Lãi</t>
   </si>
 </sst>
 </file>
@@ -565,7 +568,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -606,6 +609,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -615,9 +633,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -625,12 +640,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1012,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S189"/>
+  <dimension ref="A1:S202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="B189" sqref="B189"/>
+    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="G159" sqref="G159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1271,15 +1280,15 @@
       <c r="F13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="26" t="s">
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="K13" s="26"/>
+      <c r="K13" s="31"/>
       <c r="L13" s="16" t="s">
         <v>41</v>
       </c>
@@ -1363,11 +1372,11 @@
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
       <c r="L20" s="12"/>
-      <c r="M20" s="27" t="s">
+      <c r="M20" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="33"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
@@ -2387,11 +2396,11 @@
       <c r="F109" s="9"/>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D112" s="30" t="s">
+      <c r="D112" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="E112" s="30"/>
-      <c r="F112" s="30"/>
+      <c r="E112" s="34"/>
+      <c r="F112" s="34"/>
     </row>
     <row r="113" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B113" s="1"/>
@@ -2969,10 +2978,10 @@
       <c r="D176" s="2"/>
       <c r="E176" s="2"/>
       <c r="F176" s="2"/>
-      <c r="G176" s="31" t="s">
+      <c r="G176" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="H176" s="32"/>
+      <c r="H176" s="36"/>
     </row>
     <row r="177" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B177" s="4" t="s">
@@ -2996,7 +3005,7 @@
       <c r="E178" s="5"/>
       <c r="F178" s="5"/>
       <c r="G178" s="5"/>
-      <c r="H178" s="33" t="s">
+      <c r="H178" s="26" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3008,10 +3017,10 @@
       <c r="D179" s="5"/>
       <c r="E179" s="5"/>
       <c r="F179" s="5"/>
-      <c r="G179" s="25" t="s">
+      <c r="G179" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="H179" s="34"/>
+      <c r="H179" s="29"/>
     </row>
     <row r="180" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B180" s="4"/>
@@ -3067,7 +3076,7 @@
       <c r="E183" s="5"/>
       <c r="F183" s="5"/>
       <c r="G183" s="5"/>
-      <c r="H183" s="33" t="s">
+      <c r="H183" s="26" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3081,18 +3090,106 @@
       <c r="H184" s="9"/>
     </row>
     <row r="188" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B188" s="29" t="s">
+      <c r="B188" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="C188" s="29"/>
+      <c r="C188" s="30"/>
     </row>
     <row r="189" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
         <v>133</v>
       </c>
     </row>
+    <row r="193" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E193" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="194" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B194" s="1"/>
+      <c r="C194" s="2"/>
+      <c r="D194" s="2"/>
+      <c r="E194" s="2"/>
+      <c r="F194" s="2"/>
+      <c r="G194" s="35"/>
+      <c r="H194" s="36"/>
+    </row>
+    <row r="195" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B195" s="4"/>
+      <c r="C195" s="5"/>
+      <c r="D195" s="5"/>
+      <c r="E195" s="5"/>
+      <c r="F195" s="5"/>
+      <c r="G195" s="25"/>
+      <c r="H195" s="6"/>
+    </row>
+    <row r="196" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B196" s="4"/>
+      <c r="C196" s="5"/>
+      <c r="D196" s="5"/>
+      <c r="E196" s="5"/>
+      <c r="F196" s="5"/>
+      <c r="G196" s="5"/>
+      <c r="H196" s="27"/>
+    </row>
+    <row r="197" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B197" s="4"/>
+      <c r="C197" s="5"/>
+      <c r="D197" s="5"/>
+      <c r="E197" s="5"/>
+      <c r="F197" s="5"/>
+      <c r="G197" s="28"/>
+      <c r="H197" s="29"/>
+    </row>
+    <row r="198" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B198" s="4"/>
+      <c r="C198" s="5"/>
+      <c r="D198" s="5"/>
+      <c r="E198" s="5"/>
+      <c r="F198" s="5"/>
+      <c r="G198" s="5"/>
+      <c r="H198" s="6"/>
+    </row>
+    <row r="199" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B199" s="4"/>
+      <c r="C199" s="5"/>
+      <c r="D199" s="5"/>
+      <c r="E199" s="5"/>
+      <c r="F199" s="5"/>
+      <c r="G199" s="5"/>
+      <c r="H199" s="6"/>
+    </row>
+    <row r="200" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B200" s="4"/>
+      <c r="C200" s="5"/>
+      <c r="D200" s="5"/>
+      <c r="E200" s="5"/>
+      <c r="F200" s="5"/>
+      <c r="G200" s="25"/>
+      <c r="H200" s="6"/>
+    </row>
+    <row r="201" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B201" s="4"/>
+      <c r="C201" s="5"/>
+      <c r="D201" s="5"/>
+      <c r="E201" s="5"/>
+      <c r="F201" s="5"/>
+      <c r="G201" s="5"/>
+      <c r="H201" s="27"/>
+    </row>
+    <row r="202" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B202" s="7"/>
+      <c r="C202" s="8"/>
+      <c r="D202" s="8"/>
+      <c r="E202" s="8"/>
+      <c r="F202" s="8"/>
+      <c r="G202" s="8"/>
+      <c r="H202" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="G194:H194"/>
+    <mergeCell ref="G197:H197"/>
     <mergeCell ref="G179:H179"/>
     <mergeCell ref="B188:C188"/>
     <mergeCell ref="G13:I13"/>

</xml_diff>

<commit_message>
- update patch after comment for previous commit
</commit_message>
<xml_diff>
--- a/Tags/Document/OrderDesign.xlsx
+++ b/Tags/Document/OrderDesign.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\StockManagement\Tags\Document\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="141">
   <si>
     <t>Hóa đơn bán hàng</t>
   </si>
@@ -341,12 +336,6 @@
     <t>Tên KH</t>
   </si>
   <si>
-    <t>Xuất trong kì</t>
-  </si>
-  <si>
-    <t>Thanh toán trong kì</t>
-  </si>
-  <si>
     <t>Tồn cuối kì</t>
   </si>
   <si>
@@ -432,13 +421,34 @@
   </si>
   <si>
     <t>Báo Cáo Lỗ Lãi</t>
+  </si>
+  <si>
+    <t>Xuất trong kì (Chi from our perspective)</t>
+  </si>
+  <si>
+    <t>Thanh toán trong kì (Thu from our….)</t>
+  </si>
+  <si>
+    <t>Tồn cuối kì (Nợ cuối)</t>
+  </si>
+  <si>
+    <t>Xuất trong kì (Chi)</t>
+  </si>
+  <si>
+    <t>Thanh toán trong kì (Thu)</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>To</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -568,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -615,15 +625,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -642,6 +643,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -801,7 +813,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -836,7 +848,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1013,21 +1025,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="G159" sqref="G159"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="F149" sqref="F149"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
@@ -1047,12 +1059,12 @@
     <col min="19" max="19" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:19">
       <c r="F1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19">
       <c r="B3" s="10"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11" t="s">
@@ -1073,7 +1085,7 @@
       <c r="Q3" s="11"/>
       <c r="R3" s="12"/>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19">
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1092,7 +1104,7 @@
       <c r="Q4" s="5"/>
       <c r="R4" s="6"/>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -1117,7 +1129,7 @@
       <c r="Q5" s="5"/>
       <c r="R5" s="6"/>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19">
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
@@ -1138,7 +1150,7 @@
       <c r="Q6" s="5"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19">
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
@@ -1159,7 +1171,7 @@
       <c r="Q7" s="5"/>
       <c r="R7" s="6"/>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19">
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
@@ -1180,7 +1192,7 @@
       <c r="Q8" s="5"/>
       <c r="R8" s="6"/>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19">
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1201,7 +1213,7 @@
       <c r="Q9" s="5"/>
       <c r="R9" s="6"/>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19">
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1222,7 +1234,7 @@
       <c r="Q10" s="5"/>
       <c r="R10" s="6"/>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:19">
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1243,7 +1255,7 @@
       <c r="Q11" s="5"/>
       <c r="R11" s="6"/>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:19">
       <c r="B12" s="4" t="s">
         <v>25</v>
       </c>
@@ -1264,7 +1276,7 @@
       <c r="Q12" s="5"/>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="2:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:19" ht="45">
       <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
@@ -1280,15 +1292,15 @@
       <c r="F13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="28" t="s">
+      <c r="G13" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="31" t="s">
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="K13" s="31"/>
+      <c r="K13" s="28"/>
       <c r="L13" s="16" t="s">
         <v>41</v>
       </c>
@@ -1312,7 +1324,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:19">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1339,7 +1351,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:19">
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -1358,7 +1370,7 @@
       <c r="Q15" s="8"/>
       <c r="R15" s="9"/>
     </row>
-    <row r="20" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15" ht="30.75" customHeight="1">
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11" t="s">
@@ -1372,13 +1384,13 @@
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
       <c r="L20" s="12"/>
-      <c r="M20" s="32" t="s">
+      <c r="M20" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+    </row>
+    <row r="21" spans="2:15">
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -1391,7 +1403,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="6"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15">
       <c r="B22" s="4" t="s">
         <v>4</v>
       </c>
@@ -1406,7 +1418,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="6"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15">
       <c r="B23" s="4" t="s">
         <v>5</v>
       </c>
@@ -1421,7 +1433,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="6"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15">
       <c r="B24" s="4" t="s">
         <v>23</v>
       </c>
@@ -1436,7 +1448,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="6"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15">
       <c r="B25" s="4" t="s">
         <v>7</v>
       </c>
@@ -1451,7 +1463,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="6"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15">
       <c r="B26" s="4" t="s">
         <v>8</v>
       </c>
@@ -1466,7 +1478,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="6"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:15">
       <c r="B27" s="4" t="s">
         <v>9</v>
       </c>
@@ -1481,7 +1493,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="6"/>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:15">
       <c r="B28" s="4" t="s">
         <v>25</v>
       </c>
@@ -1496,7 +1508,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="6"/>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:15">
       <c r="B29" s="4" t="s">
         <v>10</v>
       </c>
@@ -1529,7 +1541,7 @@
       </c>
       <c r="L29" s="6"/>
     </row>
-    <row r="30" spans="2:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:15" ht="17.25" customHeight="1">
       <c r="B30" s="7"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -1548,7 +1560,7 @@
       <c r="K30" s="8"/>
       <c r="L30" s="9"/>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12">
       <c r="B34" s="10"/>
       <c r="C34" s="11"/>
       <c r="D34" s="11" t="s">
@@ -1563,7 +1575,7 @@
       <c r="K34" s="11"/>
       <c r="L34" s="12"/>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12">
       <c r="B35" s="4" t="s">
         <v>4</v>
       </c>
@@ -1578,7 +1590,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="6"/>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12">
       <c r="B36" s="4" t="s">
         <v>5</v>
       </c>
@@ -1593,7 +1605,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="6"/>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12">
       <c r="B37" s="4" t="s">
         <v>23</v>
       </c>
@@ -1608,7 +1620,7 @@
       <c r="K37" s="5"/>
       <c r="L37" s="6"/>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:12">
       <c r="B38" s="4" t="s">
         <v>7</v>
       </c>
@@ -1623,7 +1635,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="6"/>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:12">
       <c r="B39" s="4" t="s">
         <v>8</v>
       </c>
@@ -1638,7 +1650,7 @@
       <c r="K39" s="5"/>
       <c r="L39" s="6"/>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:12">
       <c r="B40" s="4" t="s">
         <v>9</v>
       </c>
@@ -1653,7 +1665,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="6"/>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:12">
       <c r="B41" s="4" t="s">
         <v>25</v>
       </c>
@@ -1668,7 +1680,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="6"/>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:12">
       <c r="B42" s="4" t="s">
         <v>10</v>
       </c>
@@ -1697,7 +1709,7 @@
       </c>
       <c r="L42" s="6"/>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:12">
       <c r="B43" s="7"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
@@ -1710,7 +1722,7 @@
       <c r="K43" s="8"/>
       <c r="L43" s="9"/>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:12">
       <c r="B46" s="10"/>
       <c r="C46" s="11"/>
       <c r="D46" s="11" t="s">
@@ -1725,7 +1737,7 @@
       <c r="K46" s="11"/>
       <c r="L46" s="12"/>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:12">
       <c r="B47" s="15"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
@@ -1738,7 +1750,7 @@
       <c r="K47" s="5"/>
       <c r="L47" s="6"/>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:12">
       <c r="B48" s="4" t="s">
         <v>4</v>
       </c>
@@ -1753,7 +1765,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="6"/>
     </row>
-    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:17">
       <c r="B49" s="4" t="s">
         <v>5</v>
       </c>
@@ -1768,7 +1780,7 @@
       <c r="K49" s="5"/>
       <c r="L49" s="6"/>
     </row>
-    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:17">
       <c r="B50" s="4" t="s">
         <v>23</v>
       </c>
@@ -1783,7 +1795,7 @@
       <c r="K50" s="5"/>
       <c r="L50" s="6"/>
     </row>
-    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:17">
       <c r="B51" s="4" t="s">
         <v>7</v>
       </c>
@@ -1798,7 +1810,7 @@
       <c r="K51" s="5"/>
       <c r="L51" s="6"/>
     </row>
-    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:17">
       <c r="B52" s="4" t="s">
         <v>8</v>
       </c>
@@ -1813,7 +1825,7 @@
       <c r="K52" s="5"/>
       <c r="L52" s="6"/>
     </row>
-    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:17">
       <c r="B53" s="4" t="s">
         <v>9</v>
       </c>
@@ -1828,7 +1840,7 @@
       <c r="K53" s="5"/>
       <c r="L53" s="6"/>
     </row>
-    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:17">
       <c r="B54" s="4" t="s">
         <v>25</v>
       </c>
@@ -1843,7 +1855,7 @@
       <c r="K54" s="5"/>
       <c r="L54" s="6"/>
     </row>
-    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:17">
       <c r="B55" s="4" t="s">
         <v>10</v>
       </c>
@@ -1872,7 +1884,7 @@
       </c>
       <c r="L55" s="6"/>
     </row>
-    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:17">
       <c r="B56" s="7"/>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
@@ -1885,7 +1897,7 @@
       <c r="K56" s="8"/>
       <c r="L56" s="9"/>
     </row>
-    <row r="59" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:17">
       <c r="B59" s="10"/>
       <c r="C59" s="11"/>
       <c r="D59" s="11" t="s">
@@ -1900,7 +1912,7 @@
       <c r="P59" s="2"/>
       <c r="Q59" s="3"/>
     </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:17">
       <c r="B60" s="4" t="s">
         <v>4</v>
       </c>
@@ -1915,7 +1927,7 @@
       <c r="P60" s="5"/>
       <c r="Q60" s="6"/>
     </row>
-    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:17">
       <c r="B61" s="4" t="s">
         <v>5</v>
       </c>
@@ -1930,7 +1942,7 @@
       <c r="P61" s="5"/>
       <c r="Q61" s="6"/>
     </row>
-    <row r="62" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:17">
       <c r="B62" s="4" t="s">
         <v>7</v>
       </c>
@@ -1945,7 +1957,7 @@
       <c r="P62" s="5"/>
       <c r="Q62" s="6"/>
     </row>
-    <row r="63" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:17">
       <c r="B63" s="4" t="s">
         <v>29</v>
       </c>
@@ -1960,7 +1972,7 @@
       <c r="P63" s="5"/>
       <c r="Q63" s="6"/>
     </row>
-    <row r="64" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:17">
       <c r="B64" s="4" t="s">
         <v>9</v>
       </c>
@@ -1974,7 +1986,7 @@
       <c r="P64" s="5"/>
       <c r="Q64" s="6"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18">
       <c r="A65" t="s">
         <v>57</v>
       </c>
@@ -1997,7 +2009,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18">
       <c r="B66" s="4" t="s">
         <v>30</v>
       </c>
@@ -2018,7 +2030,7 @@
       <c r="P66" s="5"/>
       <c r="Q66" s="6"/>
     </row>
-    <row r="67" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" ht="45">
       <c r="B67" s="21" t="s">
         <v>78</v>
       </c>
@@ -2038,7 +2050,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18">
       <c r="B68" s="22"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -2053,7 +2065,7 @@
       <c r="P68" s="5"/>
       <c r="Q68" s="5"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18">
       <c r="B70" s="10"/>
       <c r="C70" s="11"/>
       <c r="D70" s="11" t="s">
@@ -2062,7 +2074,7 @@
       <c r="E70" s="11"/>
       <c r="F70" s="12"/>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18">
       <c r="B71" s="4" t="s">
         <v>4</v>
       </c>
@@ -2071,7 +2083,7 @@
       <c r="E71" s="5"/>
       <c r="F71" s="6"/>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18">
       <c r="B72" s="4" t="s">
         <v>5</v>
       </c>
@@ -2080,7 +2092,7 @@
       <c r="E72" s="5"/>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18">
       <c r="B73" s="4" t="s">
         <v>7</v>
       </c>
@@ -2101,7 +2113,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18">
       <c r="B74" s="4" t="s">
         <v>55</v>
       </c>
@@ -2110,7 +2122,7 @@
       <c r="E74" s="5"/>
       <c r="F74" s="6"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18">
       <c r="B75" s="4" t="s">
         <v>9</v>
       </c>
@@ -2122,7 +2134,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18">
       <c r="B76" s="4" t="s">
         <v>25</v>
       </c>
@@ -2131,7 +2143,7 @@
       <c r="E76" s="5"/>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18">
       <c r="B77" s="4" t="s">
         <v>56</v>
       </c>
@@ -2146,7 +2158,7 @@
       </c>
       <c r="F77" s="6"/>
     </row>
-    <row r="78" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" ht="45">
       <c r="B78" s="21" t="s">
         <v>77</v>
       </c>
@@ -2155,7 +2167,7 @@
       <c r="E78" s="8"/>
       <c r="F78" s="9"/>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18">
       <c r="E79" t="s">
         <v>79</v>
       </c>
@@ -2172,12 +2184,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="81" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:13">
       <c r="M81" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="82" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:13">
       <c r="B82" s="1"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2" t="s">
@@ -2186,7 +2198,7 @@
       <c r="E82" s="2"/>
       <c r="F82" s="3"/>
     </row>
-    <row r="83" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:13">
       <c r="B83" s="4" t="s">
         <v>13</v>
       </c>
@@ -2195,7 +2207,7 @@
       <c r="E83" s="5"/>
       <c r="F83" s="6"/>
     </row>
-    <row r="84" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:13">
       <c r="B84" s="7" t="s">
         <v>35</v>
       </c>
@@ -2204,7 +2216,7 @@
       <c r="E84" s="8"/>
       <c r="F84" s="9"/>
     </row>
-    <row r="87" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:13">
       <c r="B87" s="1"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2" t="s">
@@ -2213,7 +2225,7 @@
       <c r="E87" s="2"/>
       <c r="F87" s="3"/>
     </row>
-    <row r="88" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:13">
       <c r="B88" s="4" t="s">
         <v>37</v>
       </c>
@@ -2222,7 +2234,7 @@
       <c r="E88" s="5"/>
       <c r="F88" s="6"/>
     </row>
-    <row r="89" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:13">
       <c r="B89" s="4" t="s">
         <v>38</v>
       </c>
@@ -2231,7 +2243,7 @@
       <c r="E89" s="5"/>
       <c r="F89" s="6"/>
     </row>
-    <row r="90" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:13">
       <c r="B90" s="4" t="s">
         <v>39</v>
       </c>
@@ -2240,7 +2252,7 @@
       <c r="E90" s="5"/>
       <c r="F90" s="6"/>
     </row>
-    <row r="91" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:13">
       <c r="B91" s="4" t="s">
         <v>40</v>
       </c>
@@ -2249,7 +2261,7 @@
       <c r="E91" s="5"/>
       <c r="F91" s="6"/>
     </row>
-    <row r="92" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:13">
       <c r="B92" s="4" t="s">
         <v>18</v>
       </c>
@@ -2258,7 +2270,7 @@
       <c r="E92" s="5"/>
       <c r="F92" s="6"/>
     </row>
-    <row r="93" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:13">
       <c r="B93" s="4" t="s">
         <v>13</v>
       </c>
@@ -2267,7 +2279,7 @@
       <c r="E93" s="5"/>
       <c r="F93" s="6"/>
     </row>
-    <row r="94" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:13">
       <c r="B94" s="4" t="s">
         <v>12</v>
       </c>
@@ -2276,7 +2288,7 @@
       <c r="E94" s="5"/>
       <c r="F94" s="6"/>
     </row>
-    <row r="95" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:13">
       <c r="B95" s="7" t="s">
         <v>24</v>
       </c>
@@ -2285,7 +2297,7 @@
       <c r="E95" s="8"/>
       <c r="F95" s="9"/>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:6">
       <c r="B98" s="1"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2" t="s">
@@ -2294,7 +2306,7 @@
       <c r="E98" s="2"/>
       <c r="F98" s="3"/>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:6">
       <c r="B99" s="4" t="s">
         <v>43</v>
       </c>
@@ -2303,7 +2315,7 @@
       <c r="E99" s="5"/>
       <c r="F99" s="6"/>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:6">
       <c r="B100" s="4" t="s">
         <v>44</v>
       </c>
@@ -2312,7 +2324,7 @@
       <c r="E100" s="5"/>
       <c r="F100" s="6"/>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:6">
       <c r="B101" s="4" t="s">
         <v>5</v>
       </c>
@@ -2321,7 +2333,7 @@
       <c r="E101" s="5"/>
       <c r="F101" s="6"/>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:6">
       <c r="B102" s="4" t="s">
         <v>45</v>
       </c>
@@ -2330,7 +2342,7 @@
       <c r="E102" s="5"/>
       <c r="F102" s="6"/>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:6">
       <c r="B103" s="4" t="s">
         <v>46</v>
       </c>
@@ -2339,7 +2351,7 @@
       <c r="E103" s="5"/>
       <c r="F103" s="6"/>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:6">
       <c r="B104" s="17" t="s">
         <v>51</v>
       </c>
@@ -2348,7 +2360,7 @@
       <c r="E104" s="5"/>
       <c r="F104" s="6"/>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:6">
       <c r="B105" s="17" t="s">
         <v>53</v>
       </c>
@@ -2357,7 +2369,7 @@
       <c r="E105" s="5"/>
       <c r="F105" s="6"/>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:6">
       <c r="B106" s="17" t="s">
         <v>54</v>
       </c>
@@ -2366,7 +2378,7 @@
       <c r="E106" s="5"/>
       <c r="F106" s="6"/>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:6">
       <c r="B107" s="4" t="s">
         <v>47</v>
       </c>
@@ -2377,7 +2389,7 @@
       <c r="E107" s="5"/>
       <c r="F107" s="6"/>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:6">
       <c r="B108" s="7" t="s">
         <v>48</v>
       </c>
@@ -2388,21 +2400,21 @@
       <c r="E108" s="8"/>
       <c r="F108" s="9"/>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:6">
       <c r="B109" s="7"/>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
       <c r="E109" s="8"/>
       <c r="F109" s="9"/>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D112" s="34" t="s">
+    <row r="112" spans="2:6">
+      <c r="D112" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="E112" s="34"/>
-      <c r="F112" s="34"/>
-    </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E112" s="31"/>
+      <c r="F112" s="31"/>
+    </row>
+    <row r="113" spans="2:8">
       <c r="B113" s="1"/>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
@@ -2415,7 +2427,7 @@
       </c>
       <c r="H113" s="3"/>
     </row>
-    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:8">
       <c r="B114" s="4"/>
       <c r="C114" s="5"/>
       <c r="D114" s="5"/>
@@ -2428,7 +2440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:8">
       <c r="B115" s="4"/>
       <c r="C115" s="5"/>
       <c r="D115" s="5"/>
@@ -2441,7 +2453,7 @@
       </c>
       <c r="H115" s="6"/>
     </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:8">
       <c r="B116" s="4"/>
       <c r="C116" s="5"/>
       <c r="D116" s="5"/>
@@ -2454,7 +2466,7 @@
       </c>
       <c r="H116" s="6"/>
     </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:8">
       <c r="B117" s="4"/>
       <c r="C117" s="5"/>
       <c r="D117" s="5"/>
@@ -2463,7 +2475,7 @@
       <c r="G117" s="5"/>
       <c r="H117" s="6"/>
     </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:8">
       <c r="B118" s="4" t="s">
         <v>84</v>
       </c>
@@ -2474,7 +2486,7 @@
       <c r="G118" s="5"/>
       <c r="H118" s="6"/>
     </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:8">
       <c r="B119" s="4" t="s">
         <v>85</v>
       </c>
@@ -2497,7 +2509,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:8">
       <c r="B120" s="7"/>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
@@ -2506,17 +2518,17 @@
       <c r="G120" s="8"/>
       <c r="H120" s="9"/>
     </row>
-    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:8">
       <c r="G122" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:8">
       <c r="E125" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:8">
       <c r="B127" s="1"/>
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
@@ -2529,7 +2541,7 @@
       </c>
       <c r="H127" s="3"/>
     </row>
-    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:8">
       <c r="B128" s="4"/>
       <c r="C128" s="5"/>
       <c r="D128" s="5"/>
@@ -2542,7 +2554,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:8">
       <c r="B129" s="4"/>
       <c r="C129" s="5"/>
       <c r="D129" s="5"/>
@@ -2555,7 +2567,7 @@
       </c>
       <c r="H129" s="6"/>
     </row>
-    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:8">
       <c r="B130" s="4"/>
       <c r="C130" s="5"/>
       <c r="D130" s="5"/>
@@ -2568,7 +2580,7 @@
       </c>
       <c r="H130" s="6"/>
     </row>
-    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:8">
       <c r="B131" s="4"/>
       <c r="C131" s="5"/>
       <c r="D131" s="5"/>
@@ -2577,7 +2589,7 @@
       <c r="G131" s="5"/>
       <c r="H131" s="6"/>
     </row>
-    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:8">
       <c r="B132" s="4" t="s">
         <v>84</v>
       </c>
@@ -2588,7 +2600,7 @@
       <c r="G132" s="5"/>
       <c r="H132" s="6"/>
     </row>
-    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:8">
       <c r="B133" s="4" t="s">
         <v>85</v>
       </c>
@@ -2608,10 +2620,10 @@
         <v>96</v>
       </c>
       <c r="H133" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="134" spans="2:8">
       <c r="B134" s="7">
         <v>1</v>
       </c>
@@ -2626,7 +2638,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:8">
       <c r="B135">
         <v>2</v>
       </c>
@@ -2637,7 +2649,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:8">
       <c r="B136">
         <v>3</v>
       </c>
@@ -2648,12 +2660,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:8">
       <c r="E138" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="139" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:8">
       <c r="B139" s="1"/>
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
@@ -2662,7 +2674,7 @@
       <c r="G139" s="2"/>
       <c r="H139" s="3"/>
     </row>
-    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:8">
       <c r="B140" s="4" t="s">
         <v>85</v>
       </c>
@@ -2673,19 +2685,19 @@
         <v>104</v>
       </c>
       <c r="E140" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F140" s="5" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="G140" s="5" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="H140" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="141" spans="2:8" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="141" spans="2:8">
       <c r="B141" s="7"/>
       <c r="C141" s="8"/>
       <c r="D141" s="8"/>
@@ -2694,14 +2706,18 @@
       <c r="G141" s="8"/>
       <c r="H141" s="9"/>
     </row>
-    <row r="144" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:8">
       <c r="E144" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="146" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B146" s="1"/>
-      <c r="C146" s="2"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="146" spans="2:8">
+      <c r="B146" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C146" s="37">
+        <v>42436</v>
+      </c>
       <c r="D146" s="2"/>
       <c r="E146" s="2"/>
       <c r="F146" s="2" t="s">
@@ -2712,9 +2728,13 @@
       </c>
       <c r="H146" s="3"/>
     </row>
-    <row r="147" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B147" s="4"/>
-      <c r="C147" s="5"/>
+    <row r="147" spans="2:8">
+      <c r="B147" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C147" s="38">
+        <v>42437</v>
+      </c>
       <c r="D147" s="5"/>
       <c r="E147" s="5"/>
       <c r="F147" s="5" t="s">
@@ -2725,7 +2745,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="148" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:8">
       <c r="B148" s="4"/>
       <c r="C148" s="5"/>
       <c r="D148" s="5"/>
@@ -2738,7 +2758,7 @@
       </c>
       <c r="H148" s="6"/>
     </row>
-    <row r="149" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:8">
       <c r="B149" s="4"/>
       <c r="C149" s="5"/>
       <c r="D149" s="5"/>
@@ -2751,7 +2771,7 @@
       </c>
       <c r="H149" s="6"/>
     </row>
-    <row r="150" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:8">
       <c r="B150" s="4"/>
       <c r="C150" s="5"/>
       <c r="D150" s="5"/>
@@ -2760,7 +2780,7 @@
       <c r="G150" s="5"/>
       <c r="H150" s="6"/>
     </row>
-    <row r="151" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:8">
       <c r="B151" s="4" t="s">
         <v>84</v>
       </c>
@@ -2771,7 +2791,7 @@
       <c r="G151" s="5"/>
       <c r="H151" s="6"/>
     </row>
-    <row r="152" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:8">
       <c r="B152" s="4" t="s">
         <v>85</v>
       </c>
@@ -2785,21 +2805,21 @@
         <v>87</v>
       </c>
       <c r="F152" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G152" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H152" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="153" spans="2:8" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="153" spans="2:8">
       <c r="B153" s="7">
         <v>1</v>
       </c>
       <c r="C153" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D153" s="8"/>
       <c r="E153" s="8"/>
@@ -2809,7 +2829,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="154" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:8">
       <c r="B154" s="4">
         <v>2</v>
       </c>
@@ -2824,7 +2844,7 @@
       </c>
       <c r="H154" s="6"/>
     </row>
-    <row r="155" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:8">
       <c r="B155" s="7">
         <v>3</v>
       </c>
@@ -2839,12 +2859,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="157" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:8">
       <c r="E157" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="158" spans="2:8" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="158" spans="2:8">
       <c r="B158" s="1"/>
       <c r="C158" s="2"/>
       <c r="D158" s="2"/>
@@ -2853,7 +2873,7 @@
       <c r="G158" s="2"/>
       <c r="H158" s="3"/>
     </row>
-    <row r="159" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:8">
       <c r="B159" s="7" t="s">
         <v>85</v>
       </c>
@@ -2864,26 +2884,26 @@
         <v>104</v>
       </c>
       <c r="E159" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F159" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="G159" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="H159" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="G159" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="H159" s="9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="164" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="164" spans="2:8">
       <c r="E164" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="165" spans="2:8" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="165" spans="2:8">
       <c r="B165" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C165" s="2"/>
       <c r="D165" s="2"/>
@@ -2892,27 +2912,27 @@
         <v>98</v>
       </c>
     </row>
-    <row r="166" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:8">
       <c r="B166" s="4" t="s">
         <v>85</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D166" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E166" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F166" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G166" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F166" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="G166" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="167" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="167" spans="2:8">
       <c r="B167" s="7"/>
       <c r="C167" s="8"/>
       <c r="D167" s="8"/>
@@ -2920,14 +2940,14 @@
       <c r="F167" s="8"/>
       <c r="G167" s="9"/>
     </row>
-    <row r="169" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:8">
       <c r="E169" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="170" spans="2:8" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="170" spans="2:8">
       <c r="B170" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C170" s="2"/>
       <c r="D170" s="2"/>
@@ -2937,27 +2957,27 @@
         <v>98</v>
       </c>
     </row>
-    <row r="171" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:8">
       <c r="B171" s="4" t="s">
         <v>85</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D171" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E171" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F171" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G171" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F171" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="G171" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="172" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="172" spans="2:8">
       <c r="B172" s="7"/>
       <c r="C172" s="8"/>
       <c r="D172" s="8"/>
@@ -2965,27 +2985,27 @@
       <c r="F172" s="8"/>
       <c r="G172" s="9"/>
     </row>
-    <row r="175" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:8">
       <c r="E175" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="176" spans="2:8" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="176" spans="2:8">
       <c r="B176" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C176" s="2"/>
       <c r="D176" s="2"/>
       <c r="E176" s="2"/>
       <c r="F176" s="2"/>
-      <c r="G176" s="35" t="s">
+      <c r="G176" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="H176" s="36"/>
-    </row>
-    <row r="177" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H176" s="33"/>
+    </row>
+    <row r="177" spans="2:8">
       <c r="B177" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C177" s="5"/>
       <c r="D177" s="5"/>
@@ -2996,9 +3016,9 @@
       </c>
       <c r="H177" s="6"/>
     </row>
-    <row r="178" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:8">
       <c r="B178" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C178" s="5"/>
       <c r="D178" s="5"/>
@@ -3009,20 +3029,20 @@
         <v>98</v>
       </c>
     </row>
-    <row r="179" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:8">
       <c r="B179" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C179" s="5"/>
       <c r="D179" s="5"/>
       <c r="E179" s="5"/>
       <c r="F179" s="5"/>
-      <c r="G179" s="28" t="s">
+      <c r="G179" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="H179" s="29"/>
-    </row>
-    <row r="180" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H179" s="35"/>
+    </row>
+    <row r="180" spans="2:8">
       <c r="B180" s="4"/>
       <c r="C180" s="5"/>
       <c r="D180" s="5"/>
@@ -3031,12 +3051,12 @@
       <c r="G180" s="5"/>
       <c r="H180" s="6"/>
     </row>
-    <row r="181" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:8">
       <c r="B181" s="4" t="s">
         <v>85</v>
       </c>
       <c r="C181" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D181" s="5" t="s">
         <v>9</v>
@@ -3054,10 +3074,10 @@
         <v>93</v>
       </c>
     </row>
-    <row r="182" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:8">
       <c r="B182" s="4"/>
       <c r="C182" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D182" s="5"/>
       <c r="E182" s="5"/>
@@ -3067,10 +3087,10 @@
       </c>
       <c r="H182" s="6"/>
     </row>
-    <row r="183" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:8">
       <c r="B183" s="4"/>
       <c r="C183" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D183" s="5"/>
       <c r="E183" s="5"/>
@@ -3080,7 +3100,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="184" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:8">
       <c r="B184" s="7"/>
       <c r="C184" s="8"/>
       <c r="D184" s="8"/>
@@ -3089,32 +3109,32 @@
       <c r="G184" s="8"/>
       <c r="H184" s="9"/>
     </row>
-    <row r="188" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B188" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="C188" s="30"/>
-    </row>
-    <row r="189" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:8">
+      <c r="B188" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="C188" s="36"/>
+    </row>
+    <row r="189" spans="2:8">
       <c r="B189" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="193" spans="2:8">
+      <c r="E193" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="193" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E193" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="194" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:8">
       <c r="B194" s="1"/>
       <c r="C194" s="2"/>
       <c r="D194" s="2"/>
       <c r="E194" s="2"/>
       <c r="F194" s="2"/>
-      <c r="G194" s="35"/>
-      <c r="H194" s="36"/>
-    </row>
-    <row r="195" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G194" s="32"/>
+      <c r="H194" s="33"/>
+    </row>
+    <row r="195" spans="2:8">
       <c r="B195" s="4"/>
       <c r="C195" s="5"/>
       <c r="D195" s="5"/>
@@ -3123,7 +3143,7 @@
       <c r="G195" s="25"/>
       <c r="H195" s="6"/>
     </row>
-    <row r="196" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:8">
       <c r="B196" s="4"/>
       <c r="C196" s="5"/>
       <c r="D196" s="5"/>
@@ -3132,16 +3152,16 @@
       <c r="G196" s="5"/>
       <c r="H196" s="27"/>
     </row>
-    <row r="197" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:8">
       <c r="B197" s="4"/>
       <c r="C197" s="5"/>
       <c r="D197" s="5"/>
       <c r="E197" s="5"/>
       <c r="F197" s="5"/>
-      <c r="G197" s="28"/>
-      <c r="H197" s="29"/>
-    </row>
-    <row r="198" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G197" s="34"/>
+      <c r="H197" s="35"/>
+    </row>
+    <row r="198" spans="2:8">
       <c r="B198" s="4"/>
       <c r="C198" s="5"/>
       <c r="D198" s="5"/>
@@ -3150,7 +3170,7 @@
       <c r="G198" s="5"/>
       <c r="H198" s="6"/>
     </row>
-    <row r="199" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:8">
       <c r="B199" s="4"/>
       <c r="C199" s="5"/>
       <c r="D199" s="5"/>
@@ -3159,7 +3179,7 @@
       <c r="G199" s="5"/>
       <c r="H199" s="6"/>
     </row>
-    <row r="200" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:8">
       <c r="B200" s="4"/>
       <c r="C200" s="5"/>
       <c r="D200" s="5"/>
@@ -3168,7 +3188,7 @@
       <c r="G200" s="25"/>
       <c r="H200" s="6"/>
     </row>
-    <row r="201" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:8">
       <c r="B201" s="4"/>
       <c r="C201" s="5"/>
       <c r="D201" s="5"/>
@@ -3177,7 +3197,7 @@
       <c r="G201" s="5"/>
       <c r="H201" s="27"/>
     </row>
-    <row r="202" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:8">
       <c r="B202" s="7"/>
       <c r="C202" s="8"/>
       <c r="D202" s="8"/>
@@ -3188,7 +3208,6 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="G194:H194"/>
     <mergeCell ref="G197:H197"/>
     <mergeCell ref="G179:H179"/>
     <mergeCell ref="B188:C188"/>
@@ -3197,6 +3216,7 @@
     <mergeCell ref="M20:O20"/>
     <mergeCell ref="D112:F112"/>
     <mergeCell ref="G176:H176"/>
+    <mergeCell ref="G194:H194"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
- Commit order design
</commit_message>
<xml_diff>
--- a/Tags/Document/OrderDesign.xlsx
+++ b/Tags/Document/OrderDesign.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\StockManagement\Tags\Document\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -10,8 +15,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="154">
   <si>
     <t>Hóa đơn bán hàng</t>
   </si>
@@ -423,12 +428,6 @@
     <t>Báo Cáo Lỗ Lãi</t>
   </si>
   <si>
-    <t>Xuất trong kì (Chi from our perspective)</t>
-  </si>
-  <si>
-    <t>Thanh toán trong kì (Thu from our….)</t>
-  </si>
-  <si>
     <t>Tồn cuối kì (Nợ cuối)</t>
   </si>
   <si>
@@ -442,13 +441,233 @@
   </si>
   <si>
     <t>To</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tồn đầu kỳ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Material History của tháng gần nhất + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tồn từ đầu tháng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>đến ngày đầu kỳ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tồn từ đầu tháng đến ngày đầu kỳ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = tổng số lượng nhập (lấy từ hóa đơn nhập mua + phiếu nhập hàng trả lại) + tổng số lượng xuất (lấy từ hóa đơn bán hàng + phiếu xuất trả nhà cung cấp) </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Chi tiết lấy từ hóa đơn nhập mua và hóa đơn bán hàng, phiếu nhập hàng trả lại (nhập), phiếu xuất trả nhà cung cấp (xuất) </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Xuất trong kỳ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = tổng số lượng xuất của vật tư lấy từ hóa đơn bán hàng + phiếu xuất trả nhà cung cấp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nhập trong kỳ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = tổng số lượng nhập của vật tư lấy từ hóa đơn nhập mua + phiếu nhập hàng trả lại</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF14BE41"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tồn cuối kỳ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tồn đầu kỳ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> nhập trong kỳ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>xuất trong kỳ</t>
+    </r>
+  </si>
+  <si>
+    <t>Giải quyết bài toán</t>
+  </si>
+  <si>
+    <t>Từ ngày</t>
+  </si>
+  <si>
+    <t>30/06/2016</t>
+  </si>
+  <si>
+    <t>Đến ngày</t>
+  </si>
+  <si>
+    <t>25/07/2016</t>
+  </si>
+  <si>
+    <t>Thực chi trong kì</t>
+  </si>
+  <si>
+    <t>Thu trong kì (Thu from our….)</t>
+  </si>
+  <si>
+    <t>Thực thu trong kì</t>
+  </si>
+  <si>
+    <t>Chi trong kì (Chi from our perspective)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,8 +690,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF14BE41"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -485,8 +718,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -574,11 +819,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -625,6 +907,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -643,23 +936,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF14BE41"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -765,6 +1079,58 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Right Arrow 16"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11277600" y="23441025"/>
+          <a:ext cx="666750" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1025,31 +1391,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S202"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="F149" sqref="F149"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="L140" sqref="L140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.28515625" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" customWidth="1"/>
     <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -1059,12 +1425,12 @@
     <col min="19" max="19" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19">
+    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="2:19">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" s="10"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11" t="s">
@@ -1085,7 +1451,7 @@
       <c r="Q3" s="11"/>
       <c r="R3" s="12"/>
     </row>
-    <row r="4" spans="2:19">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1104,7 +1470,7 @@
       <c r="Q4" s="5"/>
       <c r="R4" s="6"/>
     </row>
-    <row r="5" spans="2:19">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -1129,7 +1495,7 @@
       <c r="Q5" s="5"/>
       <c r="R5" s="6"/>
     </row>
-    <row r="6" spans="2:19">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
@@ -1150,7 +1516,7 @@
       <c r="Q6" s="5"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="2:19">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
@@ -1171,7 +1537,7 @@
       <c r="Q7" s="5"/>
       <c r="R7" s="6"/>
     </row>
-    <row r="8" spans="2:19">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
@@ -1192,7 +1558,7 @@
       <c r="Q8" s="5"/>
       <c r="R8" s="6"/>
     </row>
-    <row r="9" spans="2:19">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1213,7 +1579,7 @@
       <c r="Q9" s="5"/>
       <c r="R9" s="6"/>
     </row>
-    <row r="10" spans="2:19">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1234,7 +1600,7 @@
       <c r="Q10" s="5"/>
       <c r="R10" s="6"/>
     </row>
-    <row r="11" spans="2:19">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1255,7 +1621,7 @@
       <c r="Q11" s="5"/>
       <c r="R11" s="6"/>
     </row>
-    <row r="12" spans="2:19">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>25</v>
       </c>
@@ -1276,7 +1642,7 @@
       <c r="Q12" s="5"/>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="2:19" ht="45">
+    <row r="13" spans="2:19" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
@@ -1292,15 +1658,15 @@
       <c r="F13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="34" t="s">
+      <c r="G13" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="28" t="s">
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="K13" s="28"/>
+      <c r="K13" s="33"/>
       <c r="L13" s="16" t="s">
         <v>41</v>
       </c>
@@ -1324,7 +1690,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="2:19">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1351,7 +1717,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:19">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -1370,7 +1736,7 @@
       <c r="Q15" s="8"/>
       <c r="R15" s="9"/>
     </row>
-    <row r="20" spans="2:15" ht="30.75" customHeight="1">
+    <row r="20" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11" t="s">
@@ -1384,13 +1750,13 @@
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
       <c r="L20" s="12"/>
-      <c r="M20" s="29" t="s">
+      <c r="M20" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="N20" s="30"/>
-      <c r="O20" s="30"/>
-    </row>
-    <row r="21" spans="2:15">
+      <c r="N20" s="35"/>
+      <c r="O20" s="35"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -1403,7 +1769,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="6"/>
     </row>
-    <row r="22" spans="2:15">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>4</v>
       </c>
@@ -1418,7 +1784,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="6"/>
     </row>
-    <row r="23" spans="2:15">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>5</v>
       </c>
@@ -1433,7 +1799,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="6"/>
     </row>
-    <row r="24" spans="2:15">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>23</v>
       </c>
@@ -1448,7 +1814,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="6"/>
     </row>
-    <row r="25" spans="2:15">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>7</v>
       </c>
@@ -1463,7 +1829,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="6"/>
     </row>
-    <row r="26" spans="2:15">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>8</v>
       </c>
@@ -1478,7 +1844,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="6"/>
     </row>
-    <row r="27" spans="2:15">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>9</v>
       </c>
@@ -1493,7 +1859,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="6"/>
     </row>
-    <row r="28" spans="2:15">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>25</v>
       </c>
@@ -1508,7 +1874,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="6"/>
     </row>
-    <row r="29" spans="2:15">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>10</v>
       </c>
@@ -1541,7 +1907,7 @@
       </c>
       <c r="L29" s="6"/>
     </row>
-    <row r="30" spans="2:15" ht="17.25" customHeight="1">
+    <row r="30" spans="2:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -1560,7 +1926,7 @@
       <c r="K30" s="8"/>
       <c r="L30" s="9"/>
     </row>
-    <row r="34" spans="2:12">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="10"/>
       <c r="C34" s="11"/>
       <c r="D34" s="11" t="s">
@@ -1575,7 +1941,7 @@
       <c r="K34" s="11"/>
       <c r="L34" s="12"/>
     </row>
-    <row r="35" spans="2:12">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>4</v>
       </c>
@@ -1590,7 +1956,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="6"/>
     </row>
-    <row r="36" spans="2:12">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>5</v>
       </c>
@@ -1605,7 +1971,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="6"/>
     </row>
-    <row r="37" spans="2:12">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>23</v>
       </c>
@@ -1620,7 +1986,7 @@
       <c r="K37" s="5"/>
       <c r="L37" s="6"/>
     </row>
-    <row r="38" spans="2:12">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
         <v>7</v>
       </c>
@@ -1635,7 +2001,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="6"/>
     </row>
-    <row r="39" spans="2:12">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>8</v>
       </c>
@@ -1650,7 +2016,7 @@
       <c r="K39" s="5"/>
       <c r="L39" s="6"/>
     </row>
-    <row r="40" spans="2:12">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
         <v>9</v>
       </c>
@@ -1665,7 +2031,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="6"/>
     </row>
-    <row r="41" spans="2:12">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
         <v>25</v>
       </c>
@@ -1680,7 +2046,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="6"/>
     </row>
-    <row r="42" spans="2:12">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
         <v>10</v>
       </c>
@@ -1709,7 +2075,7 @@
       </c>
       <c r="L42" s="6"/>
     </row>
-    <row r="43" spans="2:12">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="7"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
@@ -1722,7 +2088,7 @@
       <c r="K43" s="8"/>
       <c r="L43" s="9"/>
     </row>
-    <row r="46" spans="2:12">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B46" s="10"/>
       <c r="C46" s="11"/>
       <c r="D46" s="11" t="s">
@@ -1737,7 +2103,7 @@
       <c r="K46" s="11"/>
       <c r="L46" s="12"/>
     </row>
-    <row r="47" spans="2:12">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" s="15"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
@@ -1750,7 +2116,7 @@
       <c r="K47" s="5"/>
       <c r="L47" s="6"/>
     </row>
-    <row r="48" spans="2:12">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="s">
         <v>4</v>
       </c>
@@ -1765,7 +2131,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="6"/>
     </row>
-    <row r="49" spans="2:17">
+    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
         <v>5</v>
       </c>
@@ -1780,7 +2146,7 @@
       <c r="K49" s="5"/>
       <c r="L49" s="6"/>
     </row>
-    <row r="50" spans="2:17">
+    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
         <v>23</v>
       </c>
@@ -1795,7 +2161,7 @@
       <c r="K50" s="5"/>
       <c r="L50" s="6"/>
     </row>
-    <row r="51" spans="2:17">
+    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>7</v>
       </c>
@@ -1810,7 +2176,7 @@
       <c r="K51" s="5"/>
       <c r="L51" s="6"/>
     </row>
-    <row r="52" spans="2:17">
+    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>8</v>
       </c>
@@ -1825,7 +2191,7 @@
       <c r="K52" s="5"/>
       <c r="L52" s="6"/>
     </row>
-    <row r="53" spans="2:17">
+    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>9</v>
       </c>
@@ -1840,7 +2206,7 @@
       <c r="K53" s="5"/>
       <c r="L53" s="6"/>
     </row>
-    <row r="54" spans="2:17">
+    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>25</v>
       </c>
@@ -1855,7 +2221,7 @@
       <c r="K54" s="5"/>
       <c r="L54" s="6"/>
     </row>
-    <row r="55" spans="2:17">
+    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B55" s="4" t="s">
         <v>10</v>
       </c>
@@ -1884,7 +2250,7 @@
       </c>
       <c r="L55" s="6"/>
     </row>
-    <row r="56" spans="2:17">
+    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B56" s="7"/>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
@@ -1897,7 +2263,7 @@
       <c r="K56" s="8"/>
       <c r="L56" s="9"/>
     </row>
-    <row r="59" spans="2:17">
+    <row r="59" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B59" s="10"/>
       <c r="C59" s="11"/>
       <c r="D59" s="11" t="s">
@@ -1912,7 +2278,7 @@
       <c r="P59" s="2"/>
       <c r="Q59" s="3"/>
     </row>
-    <row r="60" spans="2:17">
+    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B60" s="4" t="s">
         <v>4</v>
       </c>
@@ -1927,7 +2293,7 @@
       <c r="P60" s="5"/>
       <c r="Q60" s="6"/>
     </row>
-    <row r="61" spans="2:17">
+    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="s">
         <v>5</v>
       </c>
@@ -1942,7 +2308,7 @@
       <c r="P61" s="5"/>
       <c r="Q61" s="6"/>
     </row>
-    <row r="62" spans="2:17">
+    <row r="62" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
         <v>7</v>
       </c>
@@ -1957,7 +2323,7 @@
       <c r="P62" s="5"/>
       <c r="Q62" s="6"/>
     </row>
-    <row r="63" spans="2:17">
+    <row r="63" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
         <v>29</v>
       </c>
@@ -1972,7 +2338,7 @@
       <c r="P63" s="5"/>
       <c r="Q63" s="6"/>
     </row>
-    <row r="64" spans="2:17">
+    <row r="64" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
         <v>9</v>
       </c>
@@ -1986,7 +2352,7 @@
       <c r="P64" s="5"/>
       <c r="Q64" s="6"/>
     </row>
-    <row r="65" spans="1:18">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>57</v>
       </c>
@@ -2009,7 +2375,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="1:18">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B66" s="4" t="s">
         <v>30</v>
       </c>
@@ -2030,7 +2396,7 @@
       <c r="P66" s="5"/>
       <c r="Q66" s="6"/>
     </row>
-    <row r="67" spans="1:18" ht="45">
+    <row r="67" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="B67" s="21" t="s">
         <v>78</v>
       </c>
@@ -2050,7 +2416,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="68" spans="1:18">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B68" s="22"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -2065,7 +2431,7 @@
       <c r="P68" s="5"/>
       <c r="Q68" s="5"/>
     </row>
-    <row r="70" spans="1:18">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B70" s="10"/>
       <c r="C70" s="11"/>
       <c r="D70" s="11" t="s">
@@ -2074,7 +2440,7 @@
       <c r="E70" s="11"/>
       <c r="F70" s="12"/>
     </row>
-    <row r="71" spans="1:18">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
         <v>4</v>
       </c>
@@ -2083,7 +2449,7 @@
       <c r="E71" s="5"/>
       <c r="F71" s="6"/>
     </row>
-    <row r="72" spans="1:18">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B72" s="4" t="s">
         <v>5</v>
       </c>
@@ -2092,7 +2458,7 @@
       <c r="E72" s="5"/>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" spans="1:18">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B73" s="4" t="s">
         <v>7</v>
       </c>
@@ -2113,7 +2479,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="74" spans="1:18">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B74" s="4" t="s">
         <v>55</v>
       </c>
@@ -2122,7 +2488,7 @@
       <c r="E74" s="5"/>
       <c r="F74" s="6"/>
     </row>
-    <row r="75" spans="1:18">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
         <v>9</v>
       </c>
@@ -2134,7 +2500,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="76" spans="1:18">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B76" s="4" t="s">
         <v>25</v>
       </c>
@@ -2143,7 +2509,7 @@
       <c r="E76" s="5"/>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" spans="1:18">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B77" s="4" t="s">
         <v>56</v>
       </c>
@@ -2158,7 +2524,7 @@
       </c>
       <c r="F77" s="6"/>
     </row>
-    <row r="78" spans="1:18" ht="45">
+    <row r="78" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="B78" s="21" t="s">
         <v>77</v>
       </c>
@@ -2167,7 +2533,7 @@
       <c r="E78" s="8"/>
       <c r="F78" s="9"/>
     </row>
-    <row r="79" spans="1:18">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E79" t="s">
         <v>79</v>
       </c>
@@ -2184,12 +2550,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="81" spans="2:13">
+    <row r="81" spans="2:13" x14ac:dyDescent="0.25">
       <c r="M81" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="82" spans="2:13">
+    <row r="82" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B82" s="1"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2" t="s">
@@ -2198,7 +2564,7 @@
       <c r="E82" s="2"/>
       <c r="F82" s="3"/>
     </row>
-    <row r="83" spans="2:13">
+    <row r="83" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B83" s="4" t="s">
         <v>13</v>
       </c>
@@ -2207,7 +2573,7 @@
       <c r="E83" s="5"/>
       <c r="F83" s="6"/>
     </row>
-    <row r="84" spans="2:13">
+    <row r="84" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B84" s="7" t="s">
         <v>35</v>
       </c>
@@ -2216,7 +2582,7 @@
       <c r="E84" s="8"/>
       <c r="F84" s="9"/>
     </row>
-    <row r="87" spans="2:13">
+    <row r="87" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B87" s="1"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2" t="s">
@@ -2225,7 +2591,7 @@
       <c r="E87" s="2"/>
       <c r="F87" s="3"/>
     </row>
-    <row r="88" spans="2:13">
+    <row r="88" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B88" s="4" t="s">
         <v>37</v>
       </c>
@@ -2234,7 +2600,7 @@
       <c r="E88" s="5"/>
       <c r="F88" s="6"/>
     </row>
-    <row r="89" spans="2:13">
+    <row r="89" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B89" s="4" t="s">
         <v>38</v>
       </c>
@@ -2243,7 +2609,7 @@
       <c r="E89" s="5"/>
       <c r="F89" s="6"/>
     </row>
-    <row r="90" spans="2:13">
+    <row r="90" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B90" s="4" t="s">
         <v>39</v>
       </c>
@@ -2252,7 +2618,7 @@
       <c r="E90" s="5"/>
       <c r="F90" s="6"/>
     </row>
-    <row r="91" spans="2:13">
+    <row r="91" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B91" s="4" t="s">
         <v>40</v>
       </c>
@@ -2261,7 +2627,7 @@
       <c r="E91" s="5"/>
       <c r="F91" s="6"/>
     </row>
-    <row r="92" spans="2:13">
+    <row r="92" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B92" s="4" t="s">
         <v>18</v>
       </c>
@@ -2270,7 +2636,7 @@
       <c r="E92" s="5"/>
       <c r="F92" s="6"/>
     </row>
-    <row r="93" spans="2:13">
+    <row r="93" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="s">
         <v>13</v>
       </c>
@@ -2279,7 +2645,7 @@
       <c r="E93" s="5"/>
       <c r="F93" s="6"/>
     </row>
-    <row r="94" spans="2:13">
+    <row r="94" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B94" s="4" t="s">
         <v>12</v>
       </c>
@@ -2288,7 +2654,7 @@
       <c r="E94" s="5"/>
       <c r="F94" s="6"/>
     </row>
-    <row r="95" spans="2:13">
+    <row r="95" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B95" s="7" t="s">
         <v>24</v>
       </c>
@@ -2297,7 +2663,7 @@
       <c r="E95" s="8"/>
       <c r="F95" s="9"/>
     </row>
-    <row r="98" spans="2:6">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B98" s="1"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2" t="s">
@@ -2306,7 +2672,7 @@
       <c r="E98" s="2"/>
       <c r="F98" s="3"/>
     </row>
-    <row r="99" spans="2:6">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B99" s="4" t="s">
         <v>43</v>
       </c>
@@ -2315,7 +2681,7 @@
       <c r="E99" s="5"/>
       <c r="F99" s="6"/>
     </row>
-    <row r="100" spans="2:6">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B100" s="4" t="s">
         <v>44</v>
       </c>
@@ -2324,7 +2690,7 @@
       <c r="E100" s="5"/>
       <c r="F100" s="6"/>
     </row>
-    <row r="101" spans="2:6">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B101" s="4" t="s">
         <v>5</v>
       </c>
@@ -2333,7 +2699,7 @@
       <c r="E101" s="5"/>
       <c r="F101" s="6"/>
     </row>
-    <row r="102" spans="2:6">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B102" s="4" t="s">
         <v>45</v>
       </c>
@@ -2342,7 +2708,7 @@
       <c r="E102" s="5"/>
       <c r="F102" s="6"/>
     </row>
-    <row r="103" spans="2:6">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B103" s="4" t="s">
         <v>46</v>
       </c>
@@ -2351,7 +2717,7 @@
       <c r="E103" s="5"/>
       <c r="F103" s="6"/>
     </row>
-    <row r="104" spans="2:6">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B104" s="17" t="s">
         <v>51</v>
       </c>
@@ -2360,7 +2726,7 @@
       <c r="E104" s="5"/>
       <c r="F104" s="6"/>
     </row>
-    <row r="105" spans="2:6">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B105" s="17" t="s">
         <v>53</v>
       </c>
@@ -2369,7 +2735,7 @@
       <c r="E105" s="5"/>
       <c r="F105" s="6"/>
     </row>
-    <row r="106" spans="2:6">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B106" s="17" t="s">
         <v>54</v>
       </c>
@@ -2378,7 +2744,7 @@
       <c r="E106" s="5"/>
       <c r="F106" s="6"/>
     </row>
-    <row r="107" spans="2:6">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B107" s="4" t="s">
         <v>47</v>
       </c>
@@ -2389,7 +2755,7 @@
       <c r="E107" s="5"/>
       <c r="F107" s="6"/>
     </row>
-    <row r="108" spans="2:6">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B108" s="7" t="s">
         <v>48</v>
       </c>
@@ -2400,23 +2766,27 @@
       <c r="E108" s="8"/>
       <c r="F108" s="9"/>
     </row>
-    <row r="109" spans="2:6">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B109" s="7"/>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
       <c r="E109" s="8"/>
       <c r="F109" s="9"/>
     </row>
-    <row r="112" spans="2:6">
-      <c r="D112" s="31" t="s">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D112" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="E112" s="31"/>
-      <c r="F112" s="31"/>
-    </row>
-    <row r="113" spans="2:8">
-      <c r="B113" s="1"/>
-      <c r="C113" s="2"/>
+      <c r="E112" s="36"/>
+      <c r="F112" s="36"/>
+    </row>
+    <row r="113" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B113" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
       <c r="F113" s="2" t="s">
@@ -2426,10 +2796,28 @@
         <v>3</v>
       </c>
       <c r="H113" s="3"/>
-    </row>
-    <row r="114" spans="2:8">
-      <c r="B114" s="4"/>
-      <c r="C114" s="5"/>
+      <c r="J113" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="K113" s="40"/>
+      <c r="L113" s="40"/>
+      <c r="M113" s="40"/>
+      <c r="N113" s="40"/>
+      <c r="O113" s="40"/>
+      <c r="P113" s="40"/>
+      <c r="Q113" s="40"/>
+      <c r="R113" s="40"/>
+      <c r="S113" s="40"/>
+      <c r="T113" s="40"/>
+      <c r="U113" s="41"/>
+    </row>
+    <row r="114" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B114" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>149</v>
+      </c>
       <c r="D114" s="5"/>
       <c r="E114" s="5"/>
       <c r="F114" s="5" t="s">
@@ -2439,8 +2827,22 @@
       <c r="H114" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="115" spans="2:8">
+      <c r="J114" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="K114" s="43"/>
+      <c r="L114" s="43"/>
+      <c r="M114" s="43"/>
+      <c r="N114" s="43"/>
+      <c r="O114" s="43"/>
+      <c r="P114" s="43"/>
+      <c r="Q114" s="43"/>
+      <c r="R114" s="43"/>
+      <c r="S114" s="43"/>
+      <c r="T114" s="43"/>
+      <c r="U114" s="44"/>
+    </row>
+    <row r="115" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B115" s="4"/>
       <c r="C115" s="5"/>
       <c r="D115" s="5"/>
@@ -2452,8 +2854,22 @@
         <v>2</v>
       </c>
       <c r="H115" s="6"/>
-    </row>
-    <row r="116" spans="2:8">
+      <c r="J115" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="K115" s="46"/>
+      <c r="L115" s="46"/>
+      <c r="M115" s="46"/>
+      <c r="N115" s="46"/>
+      <c r="O115" s="46"/>
+      <c r="P115" s="46"/>
+      <c r="Q115" s="46"/>
+      <c r="R115" s="46"/>
+      <c r="S115" s="46"/>
+      <c r="T115" s="46"/>
+      <c r="U115" s="47"/>
+    </row>
+    <row r="116" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B116" s="4"/>
       <c r="C116" s="5"/>
       <c r="D116" s="5"/>
@@ -2465,8 +2881,20 @@
         <v>3</v>
       </c>
       <c r="H116" s="6"/>
-    </row>
-    <row r="117" spans="2:8">
+      <c r="J116" s="42"/>
+      <c r="K116" s="43"/>
+      <c r="L116" s="43"/>
+      <c r="M116" s="43"/>
+      <c r="N116" s="43"/>
+      <c r="O116" s="43"/>
+      <c r="P116" s="43"/>
+      <c r="Q116" s="43"/>
+      <c r="R116" s="43"/>
+      <c r="S116" s="43"/>
+      <c r="T116" s="43"/>
+      <c r="U116" s="44"/>
+    </row>
+    <row r="117" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B117" s="4"/>
       <c r="C117" s="5"/>
       <c r="D117" s="5"/>
@@ -2474,8 +2902,22 @@
       <c r="F117" s="5"/>
       <c r="G117" s="5"/>
       <c r="H117" s="6"/>
-    </row>
-    <row r="118" spans="2:8">
+      <c r="J117" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="K117" s="46"/>
+      <c r="L117" s="46"/>
+      <c r="M117" s="46"/>
+      <c r="N117" s="46"/>
+      <c r="O117" s="46"/>
+      <c r="P117" s="46"/>
+      <c r="Q117" s="46"/>
+      <c r="R117" s="46"/>
+      <c r="S117" s="46"/>
+      <c r="T117" s="46"/>
+      <c r="U117" s="47"/>
+    </row>
+    <row r="118" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B118" s="4" t="s">
         <v>84</v>
       </c>
@@ -2485,8 +2927,22 @@
       <c r="F118" s="5"/>
       <c r="G118" s="5"/>
       <c r="H118" s="6"/>
-    </row>
-    <row r="119" spans="2:8">
+      <c r="J118" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="K118" s="43"/>
+      <c r="L118" s="43"/>
+      <c r="M118" s="43"/>
+      <c r="N118" s="43"/>
+      <c r="O118" s="43"/>
+      <c r="P118" s="43"/>
+      <c r="Q118" s="43"/>
+      <c r="R118" s="43"/>
+      <c r="S118" s="43"/>
+      <c r="T118" s="43"/>
+      <c r="U118" s="44"/>
+    </row>
+    <row r="119" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B119" s="4" t="s">
         <v>85</v>
       </c>
@@ -2508,8 +2964,20 @@
       <c r="H119" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="120" spans="2:8">
+      <c r="J119" s="45"/>
+      <c r="K119" s="46"/>
+      <c r="L119" s="46"/>
+      <c r="M119" s="46"/>
+      <c r="N119" s="46"/>
+      <c r="O119" s="46"/>
+      <c r="P119" s="46"/>
+      <c r="Q119" s="46"/>
+      <c r="R119" s="46"/>
+      <c r="S119" s="46"/>
+      <c r="T119" s="46"/>
+      <c r="U119" s="47"/>
+    </row>
+    <row r="120" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B120" s="7"/>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
@@ -2517,18 +2985,48 @@
       <c r="F120" s="8"/>
       <c r="G120" s="8"/>
       <c r="H120" s="9"/>
-    </row>
-    <row r="122" spans="2:8">
+      <c r="J120" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="K120" s="43"/>
+      <c r="L120" s="43"/>
+      <c r="M120" s="43"/>
+      <c r="N120" s="43"/>
+      <c r="O120" s="43"/>
+      <c r="P120" s="43"/>
+      <c r="Q120" s="43"/>
+      <c r="R120" s="43"/>
+      <c r="S120" s="43"/>
+      <c r="T120" s="43"/>
+      <c r="U120" s="44"/>
+    </row>
+    <row r="121" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="J121" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="K121" s="46"/>
+      <c r="L121" s="46"/>
+      <c r="M121" s="46"/>
+      <c r="N121" s="46"/>
+      <c r="O121" s="46"/>
+      <c r="P121" s="46"/>
+      <c r="Q121" s="46"/>
+      <c r="R121" s="46"/>
+      <c r="S121" s="46"/>
+      <c r="T121" s="46"/>
+      <c r="U121" s="47"/>
+    </row>
+    <row r="122" spans="2:21" x14ac:dyDescent="0.25">
       <c r="G122" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="125" spans="2:8">
+    <row r="125" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E125" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="127" spans="2:8">
+    <row r="127" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B127" s="1"/>
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
@@ -2541,7 +3039,7 @@
       </c>
       <c r="H127" s="3"/>
     </row>
-    <row r="128" spans="2:8">
+    <row r="128" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B128" s="4"/>
       <c r="C128" s="5"/>
       <c r="D128" s="5"/>
@@ -2554,7 +3052,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="129" spans="2:8">
+    <row r="129" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B129" s="4"/>
       <c r="C129" s="5"/>
       <c r="D129" s="5"/>
@@ -2567,7 +3065,7 @@
       </c>
       <c r="H129" s="6"/>
     </row>
-    <row r="130" spans="2:8">
+    <row r="130" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B130" s="4"/>
       <c r="C130" s="5"/>
       <c r="D130" s="5"/>
@@ -2580,7 +3078,7 @@
       </c>
       <c r="H130" s="6"/>
     </row>
-    <row r="131" spans="2:8">
+    <row r="131" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B131" s="4"/>
       <c r="C131" s="5"/>
       <c r="D131" s="5"/>
@@ -2589,7 +3087,7 @@
       <c r="G131" s="5"/>
       <c r="H131" s="6"/>
     </row>
-    <row r="132" spans="2:8">
+    <row r="132" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B132" s="4" t="s">
         <v>84</v>
       </c>
@@ -2600,7 +3098,7 @@
       <c r="G132" s="5"/>
       <c r="H132" s="6"/>
     </row>
-    <row r="133" spans="2:8">
+    <row r="133" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B133" s="4" t="s">
         <v>85</v>
       </c>
@@ -2623,7 +3121,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="134" spans="2:8">
+    <row r="134" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B134" s="7">
         <v>1</v>
       </c>
@@ -2638,7 +3136,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="135" spans="2:8">
+    <row r="135" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B135">
         <v>2</v>
       </c>
@@ -2649,7 +3147,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="136" spans="2:8">
+    <row r="136" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B136">
         <v>3</v>
       </c>
@@ -2660,21 +3158,23 @@
         <v>98</v>
       </c>
     </row>
-    <row r="138" spans="2:8">
+    <row r="138" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E138" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="139" spans="2:8">
+    <row r="139" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B139" s="1"/>
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
       <c r="E139" s="2"/>
       <c r="F139" s="2"/>
       <c r="G139" s="2"/>
-      <c r="H139" s="3"/>
-    </row>
-    <row r="140" spans="2:8">
+      <c r="H139" s="2"/>
+      <c r="I139" s="2"/>
+      <c r="J139" s="3"/>
+    </row>
+    <row r="140" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B140" s="4" t="s">
         <v>85</v>
       </c>
@@ -2688,34 +3188,42 @@
         <v>106</v>
       </c>
       <c r="F140" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G140" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="H140" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="I140" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="J140" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="G140" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="H140" s="6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="141" spans="2:8">
+    </row>
+    <row r="141" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B141" s="7"/>
       <c r="C141" s="8"/>
       <c r="D141" s="8"/>
       <c r="E141" s="8"/>
       <c r="F141" s="8"/>
       <c r="G141" s="8"/>
-      <c r="H141" s="9"/>
-    </row>
-    <row r="144" spans="2:8">
+      <c r="H141" s="8"/>
+      <c r="I141" s="8"/>
+      <c r="J141" s="9"/>
+    </row>
+    <row r="144" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E144" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="146" spans="2:8">
+    <row r="146" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B146" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C146" s="37">
+        <v>137</v>
+      </c>
+      <c r="C146" s="28">
         <v>42436</v>
       </c>
       <c r="D146" s="2"/>
@@ -2728,11 +3236,11 @@
       </c>
       <c r="H146" s="3"/>
     </row>
-    <row r="147" spans="2:8">
+    <row r="147" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B147" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C147" s="38">
+        <v>138</v>
+      </c>
+      <c r="C147" s="29">
         <v>42437</v>
       </c>
       <c r="D147" s="5"/>
@@ -2745,7 +3253,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="148" spans="2:8">
+    <row r="148" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B148" s="4"/>
       <c r="C148" s="5"/>
       <c r="D148" s="5"/>
@@ -2758,7 +3266,7 @@
       </c>
       <c r="H148" s="6"/>
     </row>
-    <row r="149" spans="2:8">
+    <row r="149" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B149" s="4"/>
       <c r="C149" s="5"/>
       <c r="D149" s="5"/>
@@ -2771,7 +3279,7 @@
       </c>
       <c r="H149" s="6"/>
     </row>
-    <row r="150" spans="2:8">
+    <row r="150" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B150" s="4"/>
       <c r="C150" s="5"/>
       <c r="D150" s="5"/>
@@ -2780,7 +3288,7 @@
       <c r="G150" s="5"/>
       <c r="H150" s="6"/>
     </row>
-    <row r="151" spans="2:8">
+    <row r="151" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B151" s="4" t="s">
         <v>84</v>
       </c>
@@ -2791,7 +3299,7 @@
       <c r="G151" s="5"/>
       <c r="H151" s="6"/>
     </row>
-    <row r="152" spans="2:8">
+    <row r="152" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B152" s="4" t="s">
         <v>85</v>
       </c>
@@ -2814,7 +3322,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="153" spans="2:8">
+    <row r="153" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B153" s="7">
         <v>1</v>
       </c>
@@ -2829,7 +3337,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="154" spans="2:8">
+    <row r="154" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B154" s="4">
         <v>2</v>
       </c>
@@ -2844,7 +3352,7 @@
       </c>
       <c r="H154" s="6"/>
     </row>
-    <row r="155" spans="2:8">
+    <row r="155" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B155" s="7">
         <v>3</v>
       </c>
@@ -2859,12 +3367,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="157" spans="2:8">
+    <row r="157" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E157" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="158" spans="2:8">
+    <row r="158" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B158" s="1"/>
       <c r="C158" s="2"/>
       <c r="D158" s="2"/>
@@ -2873,7 +3381,7 @@
       <c r="G158" s="2"/>
       <c r="H158" s="3"/>
     </row>
-    <row r="159" spans="2:8">
+    <row r="159" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B159" s="7" t="s">
         <v>85</v>
       </c>
@@ -2887,21 +3395,21 @@
         <v>106</v>
       </c>
       <c r="F159" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G159" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H159" s="9" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="164" spans="2:8">
+    <row r="164" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E164" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="165" spans="2:8">
+    <row r="165" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B165" s="1" t="s">
         <v>115</v>
       </c>
@@ -2912,7 +3420,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="166" spans="2:8">
+    <row r="166" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B166" s="4" t="s">
         <v>85</v>
       </c>
@@ -2932,7 +3440,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="167" spans="2:8">
+    <row r="167" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B167" s="7"/>
       <c r="C167" s="8"/>
       <c r="D167" s="8"/>
@@ -2940,12 +3448,12 @@
       <c r="F167" s="8"/>
       <c r="G167" s="9"/>
     </row>
-    <row r="169" spans="2:8">
+    <row r="169" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E169" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="170" spans="2:8">
+    <row r="170" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B170" s="1" t="s">
         <v>119</v>
       </c>
@@ -2957,7 +3465,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="171" spans="2:8">
+    <row r="171" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B171" s="4" t="s">
         <v>85</v>
       </c>
@@ -2977,7 +3485,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="172" spans="2:8">
+    <row r="172" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B172" s="7"/>
       <c r="C172" s="8"/>
       <c r="D172" s="8"/>
@@ -2985,12 +3493,12 @@
       <c r="F172" s="8"/>
       <c r="G172" s="9"/>
     </row>
-    <row r="175" spans="2:8">
+    <row r="175" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E175" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="176" spans="2:8">
+    <row r="176" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B176" s="1" t="s">
         <v>124</v>
       </c>
@@ -2998,12 +3506,12 @@
       <c r="D176" s="2"/>
       <c r="E176" s="2"/>
       <c r="F176" s="2"/>
-      <c r="G176" s="32" t="s">
+      <c r="G176" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="H176" s="33"/>
-    </row>
-    <row r="177" spans="2:8">
+      <c r="H176" s="38"/>
+    </row>
+    <row r="177" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B177" s="4" t="s">
         <v>125</v>
       </c>
@@ -3016,7 +3524,7 @@
       </c>
       <c r="H177" s="6"/>
     </row>
-    <row r="178" spans="2:8">
+    <row r="178" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B178" s="4" t="s">
         <v>126</v>
       </c>
@@ -3029,7 +3537,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="179" spans="2:8">
+    <row r="179" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B179" s="4" t="s">
         <v>127</v>
       </c>
@@ -3037,12 +3545,12 @@
       <c r="D179" s="5"/>
       <c r="E179" s="5"/>
       <c r="F179" s="5"/>
-      <c r="G179" s="34" t="s">
+      <c r="G179" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="H179" s="35"/>
-    </row>
-    <row r="180" spans="2:8">
+      <c r="H179" s="31"/>
+    </row>
+    <row r="180" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B180" s="4"/>
       <c r="C180" s="5"/>
       <c r="D180" s="5"/>
@@ -3051,7 +3559,7 @@
       <c r="G180" s="5"/>
       <c r="H180" s="6"/>
     </row>
-    <row r="181" spans="2:8">
+    <row r="181" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B181" s="4" t="s">
         <v>85</v>
       </c>
@@ -3074,7 +3582,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="182" spans="2:8">
+    <row r="182" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B182" s="4"/>
       <c r="C182" s="5" t="s">
         <v>129</v>
@@ -3087,7 +3595,7 @@
       </c>
       <c r="H182" s="6"/>
     </row>
-    <row r="183" spans="2:8">
+    <row r="183" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B183" s="4"/>
       <c r="C183" s="5" t="s">
         <v>130</v>
@@ -3100,7 +3608,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="184" spans="2:8">
+    <row r="184" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B184" s="7"/>
       <c r="C184" s="8"/>
       <c r="D184" s="8"/>
@@ -3109,32 +3617,32 @@
       <c r="G184" s="8"/>
       <c r="H184" s="9"/>
     </row>
-    <row r="188" spans="2:8">
-      <c r="B188" s="36" t="s">
+    <row r="188" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B188" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="C188" s="36"/>
-    </row>
-    <row r="189" spans="2:8">
+      <c r="C188" s="32"/>
+    </row>
+    <row r="189" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="193" spans="2:8">
+    <row r="193" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E193" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="194" spans="2:8">
+    <row r="194" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B194" s="1"/>
       <c r="C194" s="2"/>
       <c r="D194" s="2"/>
       <c r="E194" s="2"/>
       <c r="F194" s="2"/>
-      <c r="G194" s="32"/>
-      <c r="H194" s="33"/>
-    </row>
-    <row r="195" spans="2:8">
+      <c r="G194" s="37"/>
+      <c r="H194" s="38"/>
+    </row>
+    <row r="195" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B195" s="4"/>
       <c r="C195" s="5"/>
       <c r="D195" s="5"/>
@@ -3143,7 +3651,7 @@
       <c r="G195" s="25"/>
       <c r="H195" s="6"/>
     </row>
-    <row r="196" spans="2:8">
+    <row r="196" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B196" s="4"/>
       <c r="C196" s="5"/>
       <c r="D196" s="5"/>
@@ -3152,16 +3660,16 @@
       <c r="G196" s="5"/>
       <c r="H196" s="27"/>
     </row>
-    <row r="197" spans="2:8">
+    <row r="197" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B197" s="4"/>
       <c r="C197" s="5"/>
       <c r="D197" s="5"/>
       <c r="E197" s="5"/>
       <c r="F197" s="5"/>
-      <c r="G197" s="34"/>
-      <c r="H197" s="35"/>
-    </row>
-    <row r="198" spans="2:8">
+      <c r="G197" s="30"/>
+      <c r="H197" s="31"/>
+    </row>
+    <row r="198" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B198" s="4"/>
       <c r="C198" s="5"/>
       <c r="D198" s="5"/>
@@ -3170,7 +3678,7 @@
       <c r="G198" s="5"/>
       <c r="H198" s="6"/>
     </row>
-    <row r="199" spans="2:8">
+    <row r="199" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B199" s="4"/>
       <c r="C199" s="5"/>
       <c r="D199" s="5"/>
@@ -3179,7 +3687,7 @@
       <c r="G199" s="5"/>
       <c r="H199" s="6"/>
     </row>
-    <row r="200" spans="2:8">
+    <row r="200" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B200" s="4"/>
       <c r="C200" s="5"/>
       <c r="D200" s="5"/>
@@ -3188,7 +3696,7 @@
       <c r="G200" s="25"/>
       <c r="H200" s="6"/>
     </row>
-    <row r="201" spans="2:8">
+    <row r="201" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B201" s="4"/>
       <c r="C201" s="5"/>
       <c r="D201" s="5"/>
@@ -3197,7 +3705,7 @@
       <c r="G201" s="5"/>
       <c r="H201" s="27"/>
     </row>
-    <row r="202" spans="2:8">
+    <row r="202" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B202" s="7"/>
       <c r="C202" s="8"/>
       <c r="D202" s="8"/>
@@ -3207,16 +3715,25 @@
       <c r="H202" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="18">
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="D112:F112"/>
+    <mergeCell ref="G176:H176"/>
+    <mergeCell ref="G194:H194"/>
+    <mergeCell ref="J113:U113"/>
+    <mergeCell ref="J114:U114"/>
+    <mergeCell ref="J115:U115"/>
+    <mergeCell ref="J116:U116"/>
+    <mergeCell ref="J117:U117"/>
+    <mergeCell ref="J118:U118"/>
+    <mergeCell ref="J119:U119"/>
+    <mergeCell ref="J120:U120"/>
+    <mergeCell ref="J121:U121"/>
     <mergeCell ref="G197:H197"/>
     <mergeCell ref="G179:H179"/>
     <mergeCell ref="B188:C188"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="J13:K13"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="D112:F112"/>
-    <mergeCell ref="G176:H176"/>
-    <mergeCell ref="G194:H194"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>